<commit_message>
Changes to resolve connection problems, ultimately coming down to a bad portname being passed
</commit_message>
<xml_diff>
--- a/Pulsar2_Commands.xlsx
+++ b/Pulsar2_Commands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13780" yWindow="1040" windowWidth="38780" windowHeight="24920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1248,7 +1248,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1865,9 +1865,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="4" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -2613,8 +2613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5856,7 +5856,7 @@
       <c r="C137" t="s">
         <v>135</v>
       </c>
-      <c r="D137">
+      <c r="D137" s="5">
         <v>1</v>
       </c>
       <c r="F137" s="10" t="s">

</xml_diff>

<commit_message>
Resolved issue of failure to get firmeare version, and several other minor bugs. Changed timeout return code. Commented out buffer-buildup diagnostic
</commit_message>
<xml_diff>
--- a/Pulsar2_Commands.xlsx
+++ b/Pulsar2_Commands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="17780" yWindow="200" windowWidth="33140" windowHeight="24820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="404">
   <si>
     <t>Command</t>
   </si>
@@ -1241,6 +1241,18 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>response 1 when it is not</t>
+  </si>
+  <si>
+    <t>usually results in no response and nErr = 3</t>
+  </si>
+  <si>
+    <t>&lt;none&gt; response coded</t>
+  </si>
+  <si>
+    <t>0 = No; 1 = Yes. Noticable delay in response</t>
   </si>
 </sst>
 </file>
@@ -1328,7 +1340,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1388,6 +1400,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -1440,7 +1458,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="401">
+  <cellStyleXfs count="409">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1842,8 +1860,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
@@ -1880,8 +1906,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="401">
+  <cellStyles count="409">
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -2080,6 +2107,10 @@
     <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
@@ -2281,6 +2312,10 @@
     <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
@@ -2611,10 +2646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N169"/>
+  <dimension ref="A1:O169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D137" sqref="D137"/>
+    <sheetView tabSelected="1" topLeftCell="E49" workbookViewId="0">
+      <selection activeCell="N159" sqref="N159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2623,7 +2658,8 @@
     <col min="2" max="2" width="28.83203125" customWidth="1"/>
     <col min="3" max="4" width="34.6640625" customWidth="1"/>
     <col min="5" max="5" width="22.83203125" customWidth="1"/>
-    <col min="6" max="7" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" customWidth="1"/>
     <col min="12" max="12" width="41" customWidth="1"/>
     <col min="13" max="13" width="18.5" customWidth="1"/>
   </cols>
@@ -2689,6 +2725,9 @@
       <c r="B4" s="17" t="s">
         <v>360</v>
       </c>
+      <c r="D4" s="26" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="B5" s="18" t="s">
@@ -2739,6 +2778,9 @@
       <c r="M8" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="N8" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
       <c r="B9" s="16" t="s">
@@ -2777,6 +2819,9 @@
       <c r="M9" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="N9" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="B10" s="16" t="s">
@@ -3255,7 +3300,7 @@
       <c r="C28" t="s">
         <v>46</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="26" t="s">
         <v>311</v>
       </c>
       <c r="E28" t="s">
@@ -3292,7 +3337,7 @@
       <c r="C31" t="s">
         <v>64</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F31" t="s">
@@ -3321,7 +3366,7 @@
       <c r="C32" t="s">
         <v>64</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F32" t="s">
@@ -3350,7 +3395,7 @@
       <c r="C33" t="s">
         <v>64</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F33" t="s">
@@ -3379,7 +3424,7 @@
       <c r="C34" t="s">
         <v>64</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F34" t="s">
@@ -3443,7 +3488,7 @@
       <c r="C36" t="s">
         <v>64</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F36" t="s">
@@ -3472,7 +3517,7 @@
       <c r="C37" t="s">
         <v>64</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F37" t="s">
@@ -3501,7 +3546,7 @@
       <c r="C38" t="s">
         <v>64</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F38" t="s">
@@ -3530,7 +3575,7 @@
       <c r="C39" t="s">
         <v>64</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F39" t="s">
@@ -3559,7 +3604,7 @@
       <c r="C40" t="s">
         <v>64</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F40" t="s">
@@ -3588,7 +3633,7 @@
       <c r="C41" t="s">
         <v>64</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F41" t="s">
@@ -3620,7 +3665,7 @@
       <c r="C42" t="s">
         <v>64</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F42" t="s">
@@ -3652,7 +3697,7 @@
       <c r="C43" t="s">
         <v>64</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F43" t="s">
@@ -3684,7 +3729,7 @@
       <c r="C44" t="s">
         <v>64</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F44" t="s">
@@ -3775,7 +3820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:15">
       <c r="B49" s="16" t="s">
         <v>104</v>
       </c>
@@ -3804,7 +3849,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:15">
       <c r="B50" s="16" t="s">
         <v>106</v>
       </c>
@@ -3839,12 +3884,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:15">
       <c r="L51" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:15">
       <c r="B52" s="16" t="s">
         <v>389</v>
       </c>
@@ -3876,17 +3921,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="17" thickBot="1">
+    <row r="54" spans="1:15" ht="17" thickBot="1">
       <c r="A54" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="17" thickTop="1" thickBot="1">
+    <row r="55" spans="1:15" ht="17" thickTop="1" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:15">
       <c r="B56" s="16" t="s">
         <v>204</v>
       </c>
@@ -3915,7 +3960,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:15">
       <c r="B57" s="16" t="s">
         <v>207</v>
       </c>
@@ -3946,8 +3991,14 @@
       <c r="M57" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="N57" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O57" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="B58" s="16" t="s">
         <v>209</v>
       </c>
@@ -3961,7 +4012,7 @@
         <v>210</v>
       </c>
       <c r="G58" t="s">
-        <v>140</v>
+        <v>403</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>12</v>
@@ -3978,8 +4029,14 @@
       <c r="M58" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="N58" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O58" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="B59" s="16" t="s">
         <v>211</v>
       </c>
@@ -4010,18 +4067,21 @@
       <c r="M59" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="N59" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:15">
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:15">
       <c r="B62" s="16" t="s">
         <v>213</v>
       </c>
@@ -4050,12 +4110,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:15">
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:15">
       <c r="B64" s="16" t="s">
         <v>109</v>
       </c>
@@ -4087,7 +4147,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="65" spans="2:13">
+    <row r="65" spans="2:14">
       <c r="B65" s="16" t="s">
         <v>112</v>
       </c>
@@ -4119,7 +4179,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="66" spans="2:13">
+    <row r="66" spans="2:14">
       <c r="B66" s="16" t="s">
         <v>114</v>
       </c>
@@ -4151,7 +4211,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="67" spans="2:13">
+    <row r="67" spans="2:14">
       <c r="B67" s="16" t="s">
         <v>115</v>
       </c>
@@ -4183,7 +4243,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="68" spans="2:13">
+    <row r="68" spans="2:14">
       <c r="B68" s="16" t="s">
         <v>120</v>
       </c>
@@ -4215,7 +4275,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="70" spans="2:13">
+    <row r="70" spans="2:14">
       <c r="B70" s="17" t="s">
         <v>126</v>
       </c>
@@ -4247,7 +4307,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="71" spans="2:13">
+    <row r="71" spans="2:14">
       <c r="B71" s="18" t="s">
         <v>125</v>
       </c>
@@ -4276,7 +4336,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="73" spans="2:13">
+    <row r="73" spans="2:14">
       <c r="B73" s="16" t="s">
         <v>129</v>
       </c>
@@ -4311,7 +4371,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="74" spans="2:13">
+    <row r="74" spans="2:14">
       <c r="B74" s="16" t="s">
         <v>134</v>
       </c>
@@ -4342,8 +4402,11 @@
       <c r="M74" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="75" spans="2:13">
+      <c r="N74" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="2:14">
       <c r="B75" s="16" t="s">
         <v>142</v>
       </c>
@@ -4375,7 +4438,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="76" spans="2:13">
+    <row r="76" spans="2:14">
       <c r="B76" s="16" t="s">
         <v>138</v>
       </c>
@@ -4410,7 +4473,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="77" spans="2:13">
+    <row r="77" spans="2:14">
       <c r="B77" s="16" t="s">
         <v>145</v>
       </c>
@@ -4442,7 +4505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="2:13">
+    <row r="78" spans="2:14">
       <c r="B78" s="17" t="s">
         <v>148</v>
       </c>
@@ -4473,8 +4536,11 @@
       <c r="M78" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="79" spans="2:13">
+      <c r="N78" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="2:14">
       <c r="G79" t="s">
         <v>152</v>
       </c>
@@ -4494,7 +4560,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="2:13">
+    <row r="80" spans="2:14">
       <c r="G80" t="s">
         <v>153</v>
       </c>
@@ -6004,7 +6070,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:14">
       <c r="B145" s="19" t="s">
         <v>249</v>
       </c>
@@ -6030,7 +6096,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:14">
       <c r="B146" s="19" t="s">
         <v>249</v>
       </c>
@@ -6059,7 +6125,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:14">
       <c r="B147" s="19" t="s">
         <v>250</v>
       </c>
@@ -6088,7 +6154,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:14">
       <c r="B148" s="19" t="s">
         <v>251</v>
       </c>
@@ -6114,7 +6180,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="149" spans="1:13">
+    <row r="149" spans="1:14">
       <c r="B149" s="19" t="s">
         <v>252</v>
       </c>
@@ -6140,7 +6206,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:14">
       <c r="B150" s="19" t="s">
         <v>253</v>
       </c>
@@ -6169,7 +6235,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:14">
       <c r="B151" s="19" t="s">
         <v>254</v>
       </c>
@@ -6195,7 +6261,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:14">
       <c r="B152" s="19" t="s">
         <v>254</v>
       </c>
@@ -6224,7 +6290,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:14">
       <c r="B153" s="19" t="s">
         <v>255</v>
       </c>
@@ -6250,7 +6316,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:14">
       <c r="B154" s="19" t="s">
         <v>256</v>
       </c>
@@ -6279,7 +6345,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:14">
       <c r="B155" s="19" t="s">
         <v>257</v>
       </c>
@@ -6308,12 +6374,12 @@
         <v>386</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="16" thickBot="1">
+    <row r="157" spans="1:14" ht="16" thickBot="1">
       <c r="A157" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:14">
       <c r="B158" s="20" t="s">
         <v>289</v>
       </c>
@@ -6345,7 +6411,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:14">
       <c r="B159" s="20" t="s">
         <v>291</v>
       </c>
@@ -6374,6 +6440,9 @@
         <v>12</v>
       </c>
       <c r="M159" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N159" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -6566,7 +6635,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6726,9 +6795,19 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
+      <c r="A14" s="23">
+        <v>43414</v>
+      </c>
+      <c r="B14" s="24">
+        <v>0.71562500000000007</v>
+      </c>
+      <c r="C14" s="24">
+        <v>0.71561342592592592</v>
+      </c>
+      <c r="D14" s="24">
+        <f>B14-C14</f>
+        <v>1.1574074074149898E-5</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="23"/>

</xml_diff>

<commit_message>
Fixed several bugs and updated the testing status in pulsar2.h
</commit_message>
<xml_diff>
--- a/Pulsar2_Commands.xlsx
+++ b/Pulsar2_Commands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17780" yWindow="200" windowWidth="33140" windowHeight="24820" tabRatio="500"/>
+    <workbookView xWindow="8180" yWindow="0" windowWidth="40540" windowHeight="24760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="402">
   <si>
     <t>Command</t>
   </si>
@@ -1241,12 +1241,6 @@
   </si>
   <si>
     <t>unknown</t>
-  </si>
-  <si>
-    <t>response 1 when it is not</t>
-  </si>
-  <si>
-    <t>usually results in no response and nErr = 3</t>
   </si>
   <si>
     <t>&lt;none&gt; response coded</t>
@@ -1458,12 +1452,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="409">
+  <cellStyleXfs count="417">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1908,7 +1910,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="409">
+  <cellStyles count="417">
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -2111,6 +2113,10 @@
     <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
@@ -2316,6 +2322,10 @@
     <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
@@ -2646,10 +2656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O169"/>
+  <dimension ref="A1:N169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E49" workbookViewId="0">
-      <selection activeCell="N159" sqref="N159"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="O60" sqref="O60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2726,7 +2736,7 @@
         <v>360</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -3056,7 +3066,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:14">
       <c r="B17" s="16" t="s">
         <v>38</v>
       </c>
@@ -3091,7 +3101,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:14">
       <c r="B18" s="16" t="s">
         <v>41</v>
       </c>
@@ -3120,12 +3130,12 @@
         <v>386</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16" thickBot="1">
+    <row r="20" spans="1:14" ht="16" thickBot="1">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:14">
       <c r="B21" s="18" t="s">
         <v>45</v>
       </c>
@@ -3154,7 +3164,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:14">
       <c r="B22" s="17" t="s">
         <v>50</v>
       </c>
@@ -3189,7 +3199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:14">
       <c r="B23" s="16" t="s">
         <v>55</v>
       </c>
@@ -3221,7 +3231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:14">
       <c r="B24" s="16" t="s">
         <v>56</v>
       </c>
@@ -3253,7 +3263,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:14">
       <c r="B25" s="16" t="s">
         <v>58</v>
       </c>
@@ -3288,12 +3298,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="16" thickBot="1">
+    <row r="27" spans="1:14" ht="16" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:14">
       <c r="B28" s="16" t="s">
         <v>61</v>
       </c>
@@ -3324,13 +3334,16 @@
       <c r="M28" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="16" thickBot="1">
+      <c r="N28" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="16" thickBot="1">
       <c r="A30" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:14">
       <c r="B31" s="16" t="s">
         <v>65</v>
       </c>
@@ -3358,8 +3371,11 @@
       <c r="M31" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="N31" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="B32" s="16" t="s">
         <v>67</v>
       </c>
@@ -3387,8 +3403,11 @@
       <c r="M32" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="B33" s="16" t="s">
         <v>69</v>
       </c>
@@ -3416,8 +3435,11 @@
       <c r="M33" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="N33" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="B34" s="16" t="s">
         <v>71</v>
       </c>
@@ -3445,8 +3467,11 @@
       <c r="M34" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="N34" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="B35" s="16" t="s">
         <v>73</v>
       </c>
@@ -3480,8 +3505,11 @@
       <c r="M35" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="N35" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="B36" s="16" t="s">
         <v>77</v>
       </c>
@@ -3509,8 +3537,11 @@
       <c r="M36" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="N36" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="B37" s="16" t="s">
         <v>79</v>
       </c>
@@ -3538,8 +3569,11 @@
       <c r="M37" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="N37" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="B38" s="16" t="s">
         <v>80</v>
       </c>
@@ -3567,8 +3601,11 @@
       <c r="M38" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="N38" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="B39" s="16" t="s">
         <v>81</v>
       </c>
@@ -3596,8 +3633,11 @@
       <c r="M39" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="N39" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="B40" s="16" t="s">
         <v>85</v>
       </c>
@@ -3626,7 +3666,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:14">
       <c r="B41" s="16" t="s">
         <v>87</v>
       </c>
@@ -3657,8 +3697,11 @@
       <c r="M41" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="N41" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="B42" s="16" t="s">
         <v>89</v>
       </c>
@@ -3689,8 +3732,11 @@
       <c r="M42" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="N42" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="B43" s="16" t="s">
         <v>90</v>
       </c>
@@ -3721,8 +3767,11 @@
       <c r="M43" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="N43" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="B44" s="16" t="s">
         <v>91</v>
       </c>
@@ -3753,13 +3802,16 @@
       <c r="M44" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" ht="16" thickBot="1">
+      <c r="N44" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="16" thickBot="1">
       <c r="A46" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:14">
       <c r="B47" s="16" t="s">
         <v>100</v>
       </c>
@@ -3788,7 +3840,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:14">
       <c r="B48" s="16" t="s">
         <v>316</v>
       </c>
@@ -3819,8 +3871,11 @@
       <c r="M48" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="N48" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="B49" s="16" t="s">
         <v>104</v>
       </c>
@@ -3849,7 +3904,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:14">
       <c r="B50" s="16" t="s">
         <v>106</v>
       </c>
@@ -3883,13 +3938,16 @@
       <c r="M50" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="N50" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="L51" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:14">
       <c r="B52" s="16" t="s">
         <v>389</v>
       </c>
@@ -3921,17 +3979,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="17" thickBot="1">
+    <row r="54" spans="1:14" ht="17" thickBot="1">
       <c r="A54" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="17" thickTop="1" thickBot="1">
+    <row r="55" spans="1:14" ht="17" thickTop="1" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:14">
       <c r="B56" s="16" t="s">
         <v>204</v>
       </c>
@@ -3960,7 +4018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:14">
       <c r="B57" s="16" t="s">
         <v>207</v>
       </c>
@@ -3994,11 +4052,8 @@
       <c r="N57" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O57" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15">
+    </row>
+    <row r="58" spans="1:14">
       <c r="B58" s="16" t="s">
         <v>209</v>
       </c>
@@ -4012,7 +4067,7 @@
         <v>210</v>
       </c>
       <c r="G58" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>12</v>
@@ -4032,11 +4087,8 @@
       <c r="N58" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O58" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15">
+    </row>
+    <row r="59" spans="1:14">
       <c r="B59" s="16" t="s">
         <v>211</v>
       </c>
@@ -4071,17 +4123,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:14">
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:14">
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:14">
       <c r="B62" s="16" t="s">
         <v>213</v>
       </c>
@@ -4109,13 +4161,16 @@
       <c r="M62" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:15">
+      <c r="N62" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:14">
       <c r="B64" s="16" t="s">
         <v>109</v>
       </c>
@@ -6408,6 +6463,9 @@
         <v>12</v>
       </c>
       <c r="M158" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N158" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -6635,7 +6693,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6810,9 +6868,19 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
+      <c r="A15" s="23">
+        <v>43415</v>
+      </c>
+      <c r="B15" s="24">
+        <v>0.67997685185185175</v>
+      </c>
+      <c r="C15" s="24">
+        <v>0.67996527777777782</v>
+      </c>
+      <c r="D15" s="24">
+        <f>B15-C15</f>
+        <v>1.1574074073927854E-5</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="23"/>

</xml_diff>

<commit_message>
switched on refraction correction and set location in connect(). The latter causes a TSX crash (always dirresnt in detail)
</commit_message>
<xml_diff>
--- a/Pulsar2_Commands.xlsx
+++ b/Pulsar2_Commands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="0" windowWidth="40540" windowHeight="24760" tabRatio="500"/>
+    <workbookView xWindow="9980" yWindow="640" windowWidth="40540" windowHeight="24760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="411">
   <si>
     <t>Command</t>
   </si>
@@ -1248,15 +1248,43 @@
   <si>
     <t>0 = No; 1 = Yes. Noticable delay in response</t>
   </si>
+  <si>
+    <t>1 byte response coded</t>
+  </si>
+  <si>
+    <t>double response coded</t>
+  </si>
+  <si>
+    <t>with 1 byte response</t>
+  </si>
+  <si>
+    <t>did do it, but CMD_FAILED 206</t>
+  </si>
+  <si>
+    <t>Cumulative error [s]</t>
+  </si>
+  <si>
+    <t>Elapsed Time [d]</t>
+  </si>
+  <si>
+    <t>Start Time [d]</t>
+  </si>
+  <si>
+    <t>End Time [d]</t>
+  </si>
+  <si>
+    <t>Drift [s/10d]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1333,8 +1361,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1396,12 +1431,29 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1451,8 +1503,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="417">
+  <cellStyleXfs count="434">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1854,6 +1921,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1871,7 +1955,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
@@ -1902,15 +1986,23 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="4"/>
+    <xf numFmtId="2" fontId="10" fillId="11" borderId="5" xfId="401" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="417">
+  <cellStyles count="434">
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -2109,14 +2201,22 @@
     <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="411" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="413" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="421" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="423" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="425" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="427" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="429" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="431" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="433" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
@@ -2318,14 +2418,23 @@
     <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="402" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="404" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="406" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="408" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="410" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="412" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="414" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="418" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="420" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="422" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="424" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="426" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="428" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="430" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="432" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="401" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
@@ -2656,10 +2765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N169"/>
+  <dimension ref="A1:O169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="O60" sqref="O60"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2735,7 +2844,7 @@
       <c r="B4" s="17" t="s">
         <v>360</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="25" t="s">
         <v>400</v>
       </c>
     </row>
@@ -2743,11 +2852,17 @@
       <c r="B5" s="18" t="s">
         <v>361</v>
       </c>
+      <c r="D5" s="26" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="B6" s="19" t="s">
         <v>362</v>
       </c>
+      <c r="D6" s="28" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="16" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -3171,7 +3286,7 @@
       <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="26" t="s">
         <v>344</v>
       </c>
       <c r="F22" t="s">
@@ -3206,7 +3321,7 @@
       <c r="C23" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="26">
         <v>1</v>
       </c>
       <c r="F23" t="s">
@@ -3238,7 +3353,7 @@
       <c r="C24" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="26">
         <v>1</v>
       </c>
       <c r="F24" t="s">
@@ -3270,7 +3385,7 @@
       <c r="C25" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="26">
         <v>1</v>
       </c>
       <c r="F25" t="s">
@@ -3310,7 +3425,7 @@
       <c r="C28" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="25" t="s">
         <v>311</v>
       </c>
       <c r="E28" t="s">
@@ -3350,7 +3465,7 @@
       <c r="C31" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F31" t="s">
@@ -3382,7 +3497,7 @@
       <c r="C32" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F32" t="s">
@@ -3407,14 +3522,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:15">
       <c r="B33" s="16" t="s">
         <v>69</v>
       </c>
       <c r="C33" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F33" t="s">
@@ -3439,14 +3554,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:15">
       <c r="B34" s="16" t="s">
         <v>71</v>
       </c>
       <c r="C34" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F34" t="s">
@@ -3471,7 +3586,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:15">
       <c r="B35" s="16" t="s">
         <v>73</v>
       </c>
@@ -3509,14 +3624,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:15">
       <c r="B36" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C36" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F36" t="s">
@@ -3541,14 +3656,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:15">
       <c r="B37" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C37" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="26" t="s">
+      <c r="D37" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F37" t="s">
@@ -3573,14 +3688,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:15">
       <c r="B38" s="16" t="s">
         <v>80</v>
       </c>
       <c r="C38" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="26" t="s">
+      <c r="D38" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F38" t="s">
@@ -3605,14 +3720,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:15">
       <c r="B39" s="16" t="s">
         <v>81</v>
       </c>
       <c r="C39" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D39" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F39" t="s">
@@ -3637,14 +3752,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:15">
       <c r="B40" s="16" t="s">
         <v>85</v>
       </c>
       <c r="C40" t="s">
         <v>64</v>
       </c>
-      <c r="D40" s="26" t="s">
+      <c r="D40" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F40" t="s">
@@ -3666,14 +3781,14 @@
         <v>397</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:15">
       <c r="B41" s="16" t="s">
         <v>87</v>
       </c>
       <c r="C41" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="26" t="s">
+      <c r="D41" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F41" t="s">
@@ -3701,14 +3816,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:15">
       <c r="B42" s="16" t="s">
         <v>89</v>
       </c>
       <c r="C42" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="26" t="s">
+      <c r="D42" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F42" t="s">
@@ -3736,14 +3851,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:15">
       <c r="B43" s="16" t="s">
         <v>90</v>
       </c>
       <c r="C43" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="26" t="s">
+      <c r="D43" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F43" t="s">
@@ -3771,14 +3886,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:15">
       <c r="B44" s="16" t="s">
         <v>91</v>
       </c>
       <c r="C44" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="26" t="s">
+      <c r="D44" s="25" t="s">
         <v>311</v>
       </c>
       <c r="F44" t="s">
@@ -3806,12 +3921,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="16" thickBot="1">
+    <row r="46" spans="1:15" ht="16" thickBot="1">
       <c r="A46" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:15">
       <c r="B47" s="16" t="s">
         <v>100</v>
       </c>
@@ -3840,14 +3955,14 @@
         <v>386</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:15">
       <c r="B48" s="16" t="s">
         <v>316</v>
       </c>
       <c r="C48" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D48" s="26">
         <v>1</v>
       </c>
       <c r="F48" t="s">
@@ -3874,8 +3989,11 @@
       <c r="N48" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:14">
+      <c r="O48" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="B49" s="16" t="s">
         <v>104</v>
       </c>
@@ -3904,14 +4022,14 @@
         <v>386</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:15">
       <c r="B50" s="16" t="s">
         <v>106</v>
       </c>
       <c r="C50" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D50" s="26">
         <v>1</v>
       </c>
       <c r="F50" t="s">
@@ -3941,20 +4059,23 @@
       <c r="N50" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="51" spans="1:14">
+      <c r="O50" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="L51" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:15">
       <c r="B52" s="16" t="s">
         <v>389</v>
       </c>
       <c r="C52" t="s">
         <v>393</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="28" t="s">
         <v>390</v>
       </c>
       <c r="F52" t="s">
@@ -3963,10 +4084,10 @@
       <c r="G52" t="s">
         <v>391</v>
       </c>
-      <c r="H52" s="25" t="s">
+      <c r="H52" s="24" t="s">
         <v>399</v>
       </c>
-      <c r="I52" s="25" t="s">
+      <c r="I52" s="24" t="s">
         <v>399</v>
       </c>
       <c r="J52" s="6" t="s">
@@ -3978,18 +4099,21 @@
       <c r="M52" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" ht="17" thickBot="1">
+      <c r="O52" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="17" thickBot="1">
       <c r="A54" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="17" thickTop="1" thickBot="1">
+    <row r="55" spans="1:15" ht="17" thickTop="1" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:15">
       <c r="B56" s="16" t="s">
         <v>204</v>
       </c>
@@ -4018,7 +4142,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:15">
       <c r="B57" s="16" t="s">
         <v>207</v>
       </c>
@@ -4053,7 +4177,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:15">
       <c r="B58" s="16" t="s">
         <v>209</v>
       </c>
@@ -4088,7 +4212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:15">
       <c r="B59" s="16" t="s">
         <v>211</v>
       </c>
@@ -4123,17 +4247,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:15">
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:15">
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:15">
       <c r="B62" s="16" t="s">
         <v>213</v>
       </c>
@@ -4165,12 +4289,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:15">
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:15">
       <c r="B64" s="16" t="s">
         <v>109</v>
       </c>
@@ -4614,6 +4738,9 @@
       <c r="M79" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="N79" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="80" spans="2:14">
       <c r="G80" t="s">
@@ -4635,7 +4762,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:14">
       <c r="G81" t="s">
         <v>154</v>
       </c>
@@ -4654,8 +4781,11 @@
       <c r="M81" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="N81" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14">
       <c r="G82" t="s">
         <v>155</v>
       </c>
@@ -4675,7 +4805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:14">
       <c r="G83" t="s">
         <v>156</v>
       </c>
@@ -4695,7 +4825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:14">
       <c r="G84" t="s">
         <v>157</v>
       </c>
@@ -4715,7 +4845,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:14">
       <c r="B85" s="18" t="s">
         <v>273</v>
       </c>
@@ -4744,7 +4874,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:14">
       <c r="B86" s="18" t="s">
         <v>269</v>
       </c>
@@ -4776,7 +4906,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:14">
       <c r="B87" s="18" t="s">
         <v>275</v>
       </c>
@@ -4805,7 +4935,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:14">
       <c r="B88" s="18" t="s">
         <v>276</v>
       </c>
@@ -4834,7 +4964,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:14">
       <c r="B90" s="17" t="s">
         <v>159</v>
       </c>
@@ -4866,7 +4996,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:14">
       <c r="B91" s="16" t="s">
         <v>160</v>
       </c>
@@ -4883,7 +5013,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:14">
       <c r="D92" t="s">
         <v>356</v>
       </c>
@@ -4891,12 +5021,12 @@
         <v>357</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="16" thickBot="1">
+    <row r="93" spans="1:14" ht="16" thickBot="1">
       <c r="A93" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:14">
       <c r="B94" s="19" t="s">
         <v>172</v>
       </c>
@@ -4922,7 +5052,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:14">
       <c r="B95" s="19" t="s">
         <v>173</v>
       </c>
@@ -4951,7 +5081,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:14">
       <c r="B96" s="19" t="s">
         <v>174</v>
       </c>
@@ -5373,7 +5503,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="113" spans="2:13">
+    <row r="113" spans="2:15">
       <c r="B113" s="16" t="s">
         <v>236</v>
       </c>
@@ -5408,7 +5538,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="114" spans="2:13">
+    <row r="114" spans="2:15">
       <c r="B114" s="16" t="s">
         <v>237</v>
       </c>
@@ -5443,7 +5573,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="115" spans="2:13">
+    <row r="115" spans="2:15">
       <c r="B115" s="16" t="s">
         <v>238</v>
       </c>
@@ -5478,7 +5608,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="117" spans="2:13">
+    <row r="117" spans="2:15">
       <c r="B117" s="19" t="s">
         <v>239</v>
       </c>
@@ -5507,7 +5637,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="118" spans="2:13">
+    <row r="118" spans="2:15">
       <c r="B118" s="19" t="s">
         <v>240</v>
       </c>
@@ -5540,7 +5670,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="120" spans="2:13">
+    <row r="120" spans="2:15">
       <c r="B120" s="19" t="s">
         <v>241</v>
       </c>
@@ -5569,7 +5699,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="121" spans="2:13">
+    <row r="121" spans="2:15">
       <c r="B121" s="19" t="s">
         <v>242</v>
       </c>
@@ -5601,7 +5731,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="122" spans="2:13">
+    <row r="122" spans="2:15">
       <c r="B122" t="s">
         <v>243</v>
       </c>
@@ -5630,7 +5760,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="123" spans="2:13">
+    <row r="123" spans="2:15">
       <c r="B123" s="19" t="s">
         <v>244</v>
       </c>
@@ -5662,11 +5792,11 @@
         <v>386</v>
       </c>
     </row>
-    <row r="124" spans="2:13">
+    <row r="124" spans="2:15">
       <c r="B124" s="16" t="s">
         <v>373</v>
       </c>
-      <c r="D124" s="5">
+      <c r="D124" s="26">
         <v>1</v>
       </c>
       <c r="F124" t="s">
@@ -5691,11 +5821,11 @@
         <v>398</v>
       </c>
     </row>
-    <row r="125" spans="2:13">
+    <row r="125" spans="2:15">
       <c r="B125" s="16" t="s">
         <v>374</v>
       </c>
-      <c r="D125" s="22">
+      <c r="D125" s="27">
         <v>1</v>
       </c>
       <c r="F125" t="s">
@@ -5719,8 +5849,14 @@
       <c r="M125" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="126" spans="2:13">
+      <c r="N125" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O125" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="126" spans="2:15">
       <c r="G126" t="s">
         <v>152</v>
       </c>
@@ -5739,8 +5875,14 @@
       <c r="M126" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="127" spans="2:13">
+      <c r="N126" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O126" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="127" spans="2:15">
       <c r="G127" t="s">
         <v>153</v>
       </c>
@@ -5760,7 +5902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="2:13">
+    <row r="128" spans="2:15">
       <c r="G128" t="s">
         <v>154</v>
       </c>
@@ -5778,6 +5920,12 @@
       </c>
       <c r="M128" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="N128" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O128" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="129" spans="1:13">
@@ -6690,20 +6838,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="14" t="s">
         <v>349</v>
       </c>
@@ -6714,7 +6864,7 @@
       </c>
       <c r="E1" s="14"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>350</v>
       </c>
@@ -6728,7 +6878,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>351</v>
       </c>
@@ -6742,7 +6892,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>352</v>
       </c>
@@ -6756,7 +6906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>353</v>
       </c>
@@ -6773,153 +6923,201 @@
         <v>238.73638888888888</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" s="14" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="14" t="s">
         <v>376</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="14" t="s">
         <v>378</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="14" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="23">
+    <row r="10" spans="1:7">
+      <c r="A10" s="22">
         <v>43410</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>0.66736111111111107</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <v>0.66736111111111107</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="23">
         <f>B10-C10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="23">
+      <c r="F10" t="s">
+        <v>406</v>
+      </c>
+      <c r="G10" s="32">
+        <f>D16*24*3600</f>
+        <v>1.0000000000065512</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="22">
         <v>43411</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <v>0.66990740740740751</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="23">
         <v>0.66990740740740751</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="23">
         <f>B11-C11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="23">
+      <c r="F11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G11" s="29">
+        <f>A10+B10</f>
+        <v>43410.667361111111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="22">
         <v>43412</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>0.66701388888888891</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="23">
         <v>0.66700231481481476</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="23">
         <f>B12-C12</f>
         <v>1.1574074074149898E-5</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="23">
+      <c r="F12" t="s">
+        <v>409</v>
+      </c>
+      <c r="G12" s="32">
+        <f>A16+B16</f>
+        <v>43417.685416666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="22">
         <v>43413</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="23">
         <v>0.67395833333333333</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="23">
         <v>0.67394675925925929</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="23">
         <f>B13-C13</f>
         <v>1.1574074074038876E-5</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="23">
+      <c r="F13" t="s">
+        <v>407</v>
+      </c>
+      <c r="G13" s="29">
+        <f>G12-G11</f>
+        <v>7.0180555555562023</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="22">
         <v>43414</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <v>0.71562500000000007</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="23">
         <v>0.71561342592592592</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="23">
         <f>B14-C14</f>
         <v>1.1574074074149898E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="23">
+    <row r="15" spans="1:7">
+      <c r="A15" s="22">
         <v>43415</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <v>0.67997685185185175</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="23">
         <v>0.67996527777777782</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="23">
         <f>B15-C15</f>
         <v>1.1574074073927854E-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
+      <c r="F15" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="G15" s="30">
+        <f>G10/G13*10</f>
+        <v>1.4248961013351487</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="22">
+        <v>43417</v>
+      </c>
+      <c r="B16" s="23">
+        <v>0.68541666666666667</v>
+      </c>
+      <c r="C16" s="23">
+        <v>0.68540509259259252</v>
+      </c>
+      <c r="D16" s="23">
+        <f>B16-C16</f>
+        <v>1.1574074074149898E-5</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
resolved all previously mentioned bugs. Added (and tested) meridian handling plus some more settings. Added more diagnostics
</commit_message>
<xml_diff>
--- a/Pulsar2_Commands.xlsx
+++ b/Pulsar2_Commands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="640" windowWidth="40540" windowHeight="24760" tabRatio="500"/>
+    <workbookView xWindow="7500" yWindow="380" windowWidth="40540" windowHeight="24760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="410">
   <si>
     <t>Command</t>
   </si>
@@ -1256,9 +1256,6 @@
   </si>
   <si>
     <t>with 1 byte response</t>
-  </si>
-  <si>
-    <t>did do it, but CMD_FAILED 206</t>
   </si>
   <si>
     <t>Cumulative error [s]</t>
@@ -1519,7 +1516,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="434">
+  <cellStyleXfs count="440">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1922,6 +1919,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2002,7 +2005,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="4"/>
     <xf numFmtId="2" fontId="10" fillId="11" borderId="5" xfId="401" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="434">
+  <cellStyles count="440">
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -2217,6 +2220,9 @@
     <cellStyle name="Followed Hyperlink" xfId="429" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="431" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="433" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="435" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="437" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="439" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
@@ -2434,6 +2440,9 @@
     <cellStyle name="Hyperlink" xfId="428" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="430" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="432" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="434" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="436" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="438" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="401" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
@@ -2767,8 +2776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="O52" sqref="O52"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="N131" sqref="N131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3377,6 +3386,9 @@
       <c r="M24" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="N24" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="25" spans="1:14">
       <c r="B25" s="16" t="s">
@@ -3412,6 +3424,9 @@
       <c r="M25" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="N25" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="27" spans="1:14" ht="16" thickBot="1">
       <c r="A27" s="3" t="s">
@@ -4099,8 +4114,8 @@
       <c r="M52" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O52" t="s">
-        <v>405</v>
+      <c r="N52" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="17" thickBot="1">
@@ -4801,8 +4816,8 @@
       <c r="K82" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M82" s="6" t="s">
-        <v>12</v>
+      <c r="M82" s="19" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="83" spans="1:14">
@@ -4821,8 +4836,8 @@
       <c r="K83" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M83" s="6" t="s">
-        <v>12</v>
+      <c r="M83" s="19" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="84" spans="1:14">
@@ -4841,8 +4856,8 @@
       <c r="K84" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M84" s="6" t="s">
-        <v>12</v>
+      <c r="M84" s="19" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="85" spans="1:14">
@@ -5944,8 +5959,8 @@
       <c r="K129" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M129" s="6" t="s">
-        <v>12</v>
+      <c r="M129" s="19" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="130" spans="1:13">
@@ -5964,8 +5979,8 @@
       <c r="K130" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M130" s="6" t="s">
-        <v>12</v>
+      <c r="M130" s="19" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="131" spans="1:13">
@@ -5984,8 +5999,8 @@
       <c r="K131" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M131" s="6" t="s">
-        <v>12</v>
+      <c r="M131" s="19" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="132" spans="1:13">
@@ -6840,8 +6855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6960,11 +6975,11 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G10" s="32">
-        <f>D16*24*3600</f>
-        <v>1.0000000000065512</v>
+        <f>D18*24*3600</f>
+        <v>1.9999999999939178</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -6982,7 +6997,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G11" s="29">
         <f>A10+B10</f>
@@ -7004,11 +7019,11 @@
         <v>1.1574074074149898E-5</v>
       </c>
       <c r="F12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G12" s="32">
-        <f>A16+B16</f>
-        <v>43417.685416666667</v>
+        <f>A18+B18</f>
+        <v>43419.669212962966</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -7026,11 +7041,11 @@
         <v>1.1574074074038876E-5</v>
       </c>
       <c r="F13" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G13" s="29">
         <f>G12-G11</f>
-        <v>7.0180555555562023</v>
+        <v>9.0018518518554629</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -7063,11 +7078,11 @@
         <v>1.1574074073927854E-5</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G15" s="30">
         <f>G10/G13*10</f>
-        <v>1.4248961013351487</v>
+        <v>2.2217650689082129</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -7085,37 +7100,57 @@
         <v>1.1574074074149898E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-    </row>
-    <row r="19" spans="1:3">
+    <row r="17" spans="1:4">
+      <c r="A17" s="22">
+        <v>43418</v>
+      </c>
+      <c r="B17" s="23">
+        <v>0.6674768518518519</v>
+      </c>
+      <c r="C17" s="23">
+        <v>0.66746527777777775</v>
+      </c>
+      <c r="D17" s="23">
+        <f>B17-C17</f>
+        <v>1.1574074074149898E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="22">
+        <v>43419</v>
+      </c>
+      <c r="B18" s="23">
+        <v>0.66921296296296295</v>
+      </c>
+      <c r="C18" s="23">
+        <v>0.66918981481481488</v>
+      </c>
+      <c r="D18" s="23">
+        <f>B18-C18</f>
+        <v>2.3148148148077752E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="23"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
     </row>

</xml_diff>

<commit_message>
Changed log entries to append. Updated test status in Pulsar2.h. Corrected spelling error in a #define. Removed redundant function prototype. Added methods to get slew rates on connection. Reordered methods in Pulsar2.cpp.
</commit_message>
<xml_diff>
--- a/Pulsar2_Commands.xlsx
+++ b/Pulsar2_Commands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40220" windowHeight="25260" tabRatio="500"/>
+    <workbookView xWindow="7780" yWindow="360" windowWidth="40220" windowHeight="25260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="413">
   <si>
     <t>Command</t>
   </si>
@@ -1539,7 +1539,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="484">
+  <cellStyleXfs count="498">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1942,6 +1942,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2082,7 +2096,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="484">
+  <cellStyles count="498">
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -2322,6 +2336,13 @@
     <cellStyle name="Followed Hyperlink" xfId="479" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="481" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="483" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="485" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="487" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="489" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="491" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="493" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="495" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="497" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
@@ -2564,6 +2585,13 @@
     <cellStyle name="Hyperlink" xfId="478" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="480" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="482" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="484" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="486" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="488" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="490" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="492" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="494" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="496" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="401" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
@@ -2897,8 +2925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="L68" sqref="L68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3089,6 +3117,9 @@
       <c r="K10" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="L10" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="B11" s="15" t="s">
@@ -3118,6 +3149,9 @@
       <c r="K11" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="L11" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" s="15" t="s">
@@ -3360,6 +3394,9 @@
       <c r="K22" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="L22" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:12">
       <c r="B23" s="15" t="s">
@@ -3386,6 +3423,9 @@
       <c r="K23" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="L23" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:12">
       <c r="B24" s="15" t="s">
@@ -4060,6 +4100,9 @@
         <v>10</v>
       </c>
       <c r="K56" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L56" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4213,8 +4256,11 @@
       <c r="I64" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K64" s="18" t="s">
-        <v>384</v>
+      <c r="K64" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L64" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="2:12">
@@ -4239,8 +4285,11 @@
       <c r="J65" t="s">
         <v>406</v>
       </c>
-      <c r="K65" s="18" t="s">
-        <v>384</v>
+      <c r="K65" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L65" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="2:12">
@@ -4265,8 +4314,11 @@
       <c r="J66" t="s">
         <v>406</v>
       </c>
-      <c r="K66" s="18" t="s">
-        <v>384</v>
+      <c r="K66" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L66" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="2:12">
@@ -4291,8 +4343,11 @@
       <c r="J67" t="s">
         <v>406</v>
       </c>
-      <c r="K67" s="18" t="s">
-        <v>384</v>
+      <c r="K67" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L67" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="2:12">
@@ -4317,7 +4372,10 @@
       <c r="J68" t="s">
         <v>406</v>
       </c>
-      <c r="K68" s="18" t="s">
+      <c r="K68" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L68" s="18" t="s">
         <v>384</v>
       </c>
     </row>
@@ -4685,8 +4743,8 @@
       <c r="J86" t="s">
         <v>270</v>
       </c>
-      <c r="K86" s="8" t="s">
-        <v>386</v>
+      <c r="K86" s="18" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -4708,8 +4766,8 @@
       <c r="I87" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K87" s="8" t="s">
-        <v>386</v>
+      <c r="K87" s="18" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -4731,8 +4789,8 @@
       <c r="I88" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K88" s="8" t="s">
-        <v>386</v>
+      <c r="K88" s="18" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -4780,6 +4838,12 @@
       <c r="J91" t="s">
         <v>161</v>
       </c>
+      <c r="K91" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="L91" s="18" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="92" spans="1:12">
       <c r="D92" t="s">
@@ -5638,8 +5702,8 @@
       <c r="J133" t="s">
         <v>270</v>
       </c>
-      <c r="K133" s="8" t="s">
-        <v>386</v>
+      <c r="K133" s="18" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="134" spans="1:12">
@@ -5662,8 +5726,8 @@
       <c r="I134" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K134" s="8" t="s">
-        <v>386</v>
+      <c r="K134" s="18" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="135" spans="1:12">
@@ -5686,8 +5750,8 @@
       <c r="I135" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K135" s="8" t="s">
-        <v>386</v>
+      <c r="K135" s="18" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="136" spans="1:12">
@@ -5719,10 +5783,10 @@
       <c r="J137" t="s">
         <v>370</v>
       </c>
-      <c r="K137" s="18" t="s">
+      <c r="K137" s="32" t="s">
         <v>385</v>
       </c>
-      <c r="L137" s="18" t="s">
+      <c r="L137" s="32" t="s">
         <v>409</v>
       </c>
     </row>
@@ -5743,6 +5807,9 @@
         <v>161</v>
       </c>
       <c r="K138" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L138" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Better setting of debug levels in every method. Set debugging level to essential. Returned logging to write instead of append. Updated the spreadsheet to record testing status.
</commit_message>
<xml_diff>
--- a/Pulsar2_Commands.xlsx
+++ b/Pulsar2_Commands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="360" windowWidth="40220" windowHeight="25260" tabRatio="500"/>
+    <workbookView xWindow="7780" yWindow="500" windowWidth="40220" windowHeight="25260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="413">
   <si>
     <t>Command</t>
   </si>
@@ -1539,7 +1539,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="498">
+  <cellStyleXfs count="504">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1942,6 +1942,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2096,7 +2102,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="498">
+  <cellStyles count="504">
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -2343,6 +2349,9 @@
     <cellStyle name="Followed Hyperlink" xfId="493" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="495" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="497" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="499" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="501" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="503" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
@@ -2592,6 +2601,9 @@
     <cellStyle name="Hyperlink" xfId="492" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="494" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="496" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="498" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="500" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="502" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="401" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
@@ -2925,8 +2937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="L68" sqref="L68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L127" sqref="L127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4578,6 +4590,9 @@
       <c r="K77" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="L77" s="18" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="78" spans="2:12">
       <c r="B78" s="16" t="s">
@@ -4638,6 +4653,9 @@
       <c r="K80" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="L80" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="81" spans="1:12">
       <c r="G81" t="s">
@@ -5587,6 +5605,9 @@
         <v>10</v>
       </c>
       <c r="K127" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L127" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>